<commit_message>
Add in full activity definitions
</commit_message>
<xml_diff>
--- a/source_data/cross_over_1.xlsx
+++ b/source_data/cross_over_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068C1570-5B7C-BD4A-8FDD-CFD0B4467239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3802D5D-5BD3-E14E-858A-59BD8C3FC979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50700" yWindow="500" windowWidth="42420" windowHeight="24980" firstSheet="3" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="50700" yWindow="500" windowWidth="42420" windowHeight="24980" firstSheet="3" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="studyDesignArms" sheetId="15" r:id="rId4"/>
     <sheet name="studyDesignEpochs" sheetId="14" r:id="rId5"/>
     <sheet name="mainTimeline" sheetId="1" r:id="rId6"/>
-    <sheet name="studyDesignII" sheetId="6" r:id="rId7"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId8"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId9"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId10"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId11"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId12"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId13"/>
-    <sheet name="configuration" sheetId="10" r:id="rId14"/>
+    <sheet name="studyDesignActivities" sheetId="16" r:id="rId7"/>
+    <sheet name="studyDesignII" sheetId="6" r:id="rId8"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId9"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId10"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId11"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId12"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId13"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId14"/>
+    <sheet name="configuration" sheetId="10" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="323">
   <si>
     <t>Epoch</t>
   </si>
@@ -970,13 +971,61 @@
   </si>
   <si>
     <t>Discharge</t>
+  </si>
+  <si>
+    <t>Randomization</t>
+  </si>
+  <si>
+    <t>All eligibility criteria met</t>
+  </si>
+  <si>
+    <t>At the discretion of the investigator</t>
+  </si>
+  <si>
+    <t>Hypoglycemic Events</t>
+  </si>
+  <si>
+    <t>Concomitant Medication</t>
+  </si>
+  <si>
+    <t>Stopped once bedside PG is &lt;60 mg/dL</t>
+  </si>
+  <si>
+    <t>5 minutes after bedside PG reaches &lt;60 mg/dL and insulin infusion is stopped.</t>
+  </si>
+  <si>
+    <t>At periods 1 and 2 pts should have fasted at least 8 hoours before any study procedures</t>
+  </si>
+  <si>
+    <t>Serum Pregnancy Tests</t>
+  </si>
+  <si>
+    <t>Only females of childbearing potential</t>
+  </si>
+  <si>
+    <t>Only Females when needed to confirm postmenopausal status</t>
+  </si>
+  <si>
+    <t>activityName</t>
+  </si>
+  <si>
+    <t>activityDescription</t>
+  </si>
+  <si>
+    <t>activityIsConditional</t>
+  </si>
+  <si>
+    <t>activityIsConditionalReason</t>
+  </si>
+  <si>
+    <t>For IMG only</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1028,6 +1077,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1061,7 +1124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1142,6 +1205,11 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1716,6 +1784,416 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="59.5" customWidth="1"/>
+    <col min="6" max="7" width="31.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -1826,11 +2304,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D608A778-255D-4443-A7EA-03049F1FC98F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1931,7 +2409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -2100,7 +2578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -2224,7 +2702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2700,7 +3178,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3354,6 +3832,417 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81EA128-B7FE-1C45-9311-422BAF2D7A28}">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="55.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="68.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="33"/>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="C14" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="C16" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="26" t="s">
+        <v>290</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>292</v>
+      </c>
+      <c r="C23" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>252</v>
+      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="C25" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>293</v>
+      </c>
+      <c r="C27" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>295</v>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>296</v>
+      </c>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>297</v>
+      </c>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+    </row>
+    <row r="35" spans="1:4" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3442,7 +4331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -3532,414 +4421,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
-  <dimension ref="A1:G36"/>
-  <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="44" customWidth="1"/>
-    <col min="3" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="59.5" customWidth="1"/>
-    <col min="6" max="7" width="31.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Tweaks to cross over study
</commit_message>
<xml_diff>
--- a/source_data/cross_over_1.xlsx
+++ b/source_data/cross_over_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323F14F9-0DDB-F140-AEDA-E096AAF5420B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4056A139-773B-0946-B2EF-235168C6938E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15880" yWindow="500" windowWidth="51180" windowHeight="24980" firstSheet="2" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -2968,7 +2968,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add detail to study definition
</commit_message>
<xml_diff>
--- a/source_data/cross_over_1.xlsx
+++ b/source_data/cross_over_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4056A139-773B-0946-B2EF-235168C6938E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81F7FA4-ED53-0B42-8221-021DB49898FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15880" yWindow="500" windowWidth="51180" windowHeight="24980" firstSheet="2" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="49340" yWindow="500" windowWidth="51180" windowHeight="24980" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="347">
   <si>
     <t>Epoch</t>
   </si>
@@ -152,18 +152,6 @@
     <t>DUNS</t>
   </si>
   <si>
-    <t>123456789</t>
-  </si>
-  <si>
-    <t>ACME Pharma</t>
-  </si>
-  <si>
-    <t>AP1234</t>
-  </si>
-  <si>
-    <t>Somewhere|In a City|In a District|In a big state|12345|FRA</t>
-  </si>
-  <si>
     <t>organisationAddress</t>
   </si>
   <si>
@@ -752,9 +740,6 @@
     <t>Cross Over</t>
   </si>
   <si>
-    <t>Test of a cross over</t>
-  </si>
-  <si>
     <t>Period 1</t>
   </si>
   <si>
@@ -1077,13 +1062,44 @@
   </si>
   <si>
     <t>dayOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Phase 3 Study of Nasal Glucagon (LY900018) Compared to Intramuscular Glucagon for Treatment of
+Insulin-induced Hypoglycemia in Japanese Patients with Diabetes Mellitus </t>
+  </si>
+  <si>
+    <t>LY900018</t>
+  </si>
+  <si>
+    <t>5-1-28, ISOGAMIDORI, CHUO-KU LILLY PLAZA ONE BLDG|KOBE|HYOGO||651-0086|JP</t>
+  </si>
+  <si>
+    <t>Eli Lilly Japan K.K</t>
+  </si>
+  <si>
+    <t>006421325</t>
+  </si>
+  <si>
+    <t>NCT03421379</t>
+  </si>
+  <si>
+    <t>USGOV</t>
+  </si>
+  <si>
+    <t>CT-GOV</t>
+  </si>
+  <si>
+    <t>ClinicalTrials.gov</t>
+  </si>
+  <si>
+    <t>Study Registry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1149,6 +1165,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1182,7 +1204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1250,18 +1272,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1269,9 +1279,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1283,6 +1290,22 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1600,8 +1623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1620,7 +1643,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1648,7 +1671,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -1662,7 +1685,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1673,10 +1696,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -1687,10 +1710,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -1701,7 +1724,7 @@
     </row>
     <row r="7" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="10"/>
@@ -1723,42 +1746,42 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="F9" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="G9" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="H9" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="16" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="D10" s="10" t="s">
         <v>129</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>133</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1768,7 +1791,7 @@
         <v>45047</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1875,72 +1898,72 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>57</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1967,205 +1990,205 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B1" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2378,90 +2401,90 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
         <v>114</v>
       </c>
-      <c r="B2" t="s">
-        <v>118</v>
-      </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" t="s">
         <v>116</v>
       </c>
-      <c r="E2" t="s">
-        <v>120</v>
-      </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" t="s">
         <v>145</v>
-      </c>
-      <c r="B5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H5" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2490,82 +2513,82 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E3" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E4" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="31" t="s">
-        <v>303</v>
+      <c r="E5" s="27" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2594,147 +2617,147 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>167</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2761,104 +2784,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2882,18 +2905,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2903,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2915,7 +2938,7 @@
     <col min="2" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="52.5" customWidth="1"/>
+    <col min="6" max="6" width="72.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -2935,7 +2958,7 @@
         <v>21</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2943,19 +2966,36 @@
         <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
+        <v>341</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>340</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>338</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3" t="s">
+        <v>346</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2967,7 +3007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
@@ -2980,127 +3020,127 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+        <v>203</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+        <v>204</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="B4" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
+      <c r="B5" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
+      <c r="B6" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
+      <c r="B7" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="B8" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+        <v>147</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>341</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+        <v>148</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>336</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>25</v>
@@ -3111,19 +3151,19 @@
         <v>22</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3131,19 +3171,19 @@
         <v>23</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -3160,16 +3200,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3194,19 +3234,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>220</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3214,16 +3254,16 @@
         <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -3234,13 +3274,13 @@
         <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3268,13 +3308,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3282,43 +3322,43 @@
         <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -3326,10 +3366,10 @@
         <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -3359,10 +3399,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>0</v>
@@ -3370,27 +3410,27 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="30" t="s">
-        <v>234</v>
-      </c>
-      <c r="F1" s="30"/>
+      <c r="E1" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="38"/>
       <c r="G1" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="I1" s="30"/>
+        <v>230</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" s="38"/>
       <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>2</v>
@@ -3405,10 +3445,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>8</v>
@@ -3456,71 +3496,71 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -3531,7 +3571,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -3539,10 +3579,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
@@ -3559,7 +3599,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C11"/>
       <c r="D11" s="2"/>
@@ -3574,10 +3614,10 @@
     </row>
     <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="26" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C12" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>5</v>
@@ -3588,10 +3628,10 @@
     </row>
     <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="26" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="C13" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>5</v>
@@ -3602,7 +3642,7 @@
     </row>
     <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="26" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C14"/>
       <c r="D14" s="1" t="s">
@@ -3611,7 +3651,7 @@
     </row>
     <row r="15" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B15" s="26" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="1" t="s">
@@ -3635,10 +3675,10 @@
     </row>
     <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="26" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C16" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>5</v>
@@ -3655,10 +3695,10 @@
     </row>
     <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="26" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C17" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>5</v>
@@ -3666,10 +3706,10 @@
     </row>
     <row r="18" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="26" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C18" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>5</v>
@@ -3683,7 +3723,7 @@
     </row>
     <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="26" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C19"/>
       <c r="F19" s="1" t="s">
@@ -3695,7 +3735,7 @@
     </row>
     <row r="20" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="26" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C20"/>
       <c r="D20" s="1" t="s">
@@ -3721,11 +3761,11 @@
       </c>
     </row>
     <row r="21" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B21" s="39" t="s">
-        <v>281</v>
+      <c r="B21" s="34" t="s">
+        <v>276</v>
       </c>
       <c r="C21" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>5</v>
@@ -3735,8 +3775,8 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B22" s="39" t="s">
-        <v>283</v>
+      <c r="B22" s="34" t="s">
+        <v>278</v>
       </c>
       <c r="C22"/>
       <c r="F22" s="1" t="s">
@@ -3747,8 +3787,8 @@
       </c>
     </row>
     <row r="23" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B23" s="39" t="s">
-        <v>284</v>
+      <c r="B23" s="34" t="s">
+        <v>279</v>
       </c>
       <c r="C23"/>
       <c r="F23" s="1" t="s">
@@ -3759,8 +3799,8 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B24" s="39" t="s">
-        <v>285</v>
+      <c r="B24" s="34" t="s">
+        <v>280</v>
       </c>
       <c r="C24"/>
       <c r="F24" s="1" t="s">
@@ -3772,10 +3812,10 @@
     </row>
     <row r="25" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C25" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>5</v>
@@ -3786,10 +3826,10 @@
     </row>
     <row r="26" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="26" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C26" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>5</v>
@@ -3800,7 +3840,7 @@
     </row>
     <row r="27" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="26" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C27"/>
       <c r="D27" s="1" t="s">
@@ -3812,12 +3852,12 @@
     </row>
     <row r="28" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B28" s="26" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="26" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>5</v>
@@ -3825,7 +3865,7 @@
     </row>
     <row r="30" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" s="26" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>5</v>
@@ -3836,7 +3876,7 @@
     </row>
     <row r="31" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="26" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>5</v>
@@ -3844,7 +3884,7 @@
     </row>
     <row r="32" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="26" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>5</v>
@@ -3861,7 +3901,7 @@
     </row>
     <row r="33" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B33" s="26" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>5</v>
@@ -3869,7 +3909,7 @@
     </row>
     <row r="34" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="26" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>5</v>
@@ -3877,7 +3917,7 @@
     </row>
     <row r="35" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="26" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>5</v>
@@ -3885,7 +3925,7 @@
     </row>
     <row r="36" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="26" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>5</v>
@@ -3893,12 +3933,12 @@
     </row>
     <row r="37" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B37" s="26" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B38" s="26" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>5</v>
@@ -3906,7 +3946,7 @@
     </row>
     <row r="39" spans="2:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B39" s="26" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>5</v>
@@ -3914,7 +3954,7 @@
     </row>
     <row r="40" spans="2:10" ht="34" x14ac:dyDescent="0.2">
       <c r="B40" s="26" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>5</v>
@@ -3951,56 +3991,56 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
     </row>
     <row r="2" spans="1:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
@@ -4008,15 +4048,15 @@
       <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
@@ -4024,15 +4064,15 @@
       <c r="C5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="6" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
@@ -4040,80 +4080,80 @@
       <c r="C6" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="L6" s="33" t="s">
+        <v>335</v>
+      </c>
+      <c r="M6" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="N6" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="O6" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="P6" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q6" s="33" t="s">
         <v>328</v>
       </c>
-      <c r="E6" s="38" t="s">
-        <v>325</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>326</v>
-      </c>
-      <c r="G6" s="38" t="s">
-        <v>327</v>
-      </c>
-      <c r="H6" s="38" t="s">
-        <v>339</v>
-      </c>
-      <c r="I6" s="38" t="s">
-        <v>323</v>
-      </c>
-      <c r="J6" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="K6" s="38" t="s">
-        <v>324</v>
-      </c>
-      <c r="L6" s="38" t="s">
-        <v>340</v>
-      </c>
-      <c r="M6" s="38" t="s">
+      <c r="R6" s="33" t="s">
         <v>329</v>
       </c>
-      <c r="N6" s="38" t="s">
+      <c r="S6" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="O6" s="38" t="s">
+      <c r="T6" s="33" t="s">
         <v>331</v>
-      </c>
-      <c r="P6" s="38" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q6" s="38" t="s">
-        <v>333</v>
-      </c>
-      <c r="R6" s="38" t="s">
-        <v>334</v>
-      </c>
-      <c r="S6" s="38" t="s">
-        <v>335</v>
-      </c>
-      <c r="T6" s="38" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+        <v>178</v>
+      </c>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
@@ -4123,15 +4163,15 @@
         <v>7</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="26" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C10" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -4155,10 +4195,10 @@
     </row>
     <row r="11" spans="1:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="26" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C11" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>5</v>
@@ -4182,7 +4222,7 @@
     </row>
     <row r="12" spans="1:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="26" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="7" t="s">
@@ -4209,7 +4249,7 @@
     </row>
     <row r="13" spans="1:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="26" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="7" t="s">
@@ -4236,10 +4276,10 @@
     </row>
     <row r="14" spans="1:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="26" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C14" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>5</v>
@@ -4275,7 +4315,7 @@
     </row>
     <row r="15" spans="1:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="26" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
@@ -4313,7 +4353,7 @@
     </row>
     <row r="16" spans="1:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="26" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>5</v>
@@ -4337,7 +4377,7 @@
     </row>
     <row r="17" spans="2:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="26" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>5</v>
@@ -4361,7 +4401,7 @@
     </row>
     <row r="18" spans="2:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="26" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>5</v>
@@ -4411,7 +4451,7 @@
     </row>
     <row r="19" spans="2:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="26" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>5</v>
@@ -4461,7 +4501,7 @@
     </row>
     <row r="20" spans="2:20" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="26" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>5</v>
@@ -4487,7 +4527,7 @@
     </row>
     <row r="21" spans="2:20" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" s="13" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>5</v>
@@ -4507,7 +4547,7 @@
     </row>
     <row r="22" spans="2:20" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B22" s="26" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>5</v>
@@ -4554,393 +4594,393 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>270</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>270</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+        <v>265</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>306</v>
-      </c>
-      <c r="C3" s="33" t="b">
+        <v>266</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>307</v>
+      <c r="D3" s="29" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>272</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>272</v>
-      </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
+        <v>267</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
-        <v>273</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="C5" s="33" t="b">
+        <v>268</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="C5" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>308</v>
+      <c r="D5" s="29" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>274</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+        <v>269</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>275</v>
-      </c>
-      <c r="D7" s="33"/>
+        <v>270</v>
+      </c>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>276</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>276</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
+        <v>271</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
-        <v>277</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
+        <v>272</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>278</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
+        <v>273</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
-        <v>279</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>309</v>
-      </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
+        <v>274</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>310</v>
-      </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
+        <v>275</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>281</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
+        <v>276</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>283</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="C14" s="33" t="b">
+        <v>278</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="C14" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>311</v>
+      <c r="D14" s="29" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>284</v>
-      </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
+        <v>279</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>285</v>
-      </c>
-      <c r="C16" s="33" t="b">
+        <v>280</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="C16" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>312</v>
+      <c r="D16" s="29" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>286</v>
-      </c>
-      <c r="C17" s="33" t="b">
+        <v>281</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="C17" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="D17" s="33" t="s">
-        <v>321</v>
+      <c r="D17" s="29" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
-        <v>287</v>
-      </c>
-      <c r="B18" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
+        <v>282</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>288</v>
-      </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
+        <v>283</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
-        <v>289</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>289</v>
-      </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
+        <v>284</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>290</v>
-      </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
+        <v>285</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>291</v>
-      </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
+        <v>286</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>292</v>
-      </c>
-      <c r="C23" s="33" t="b">
+        <v>287</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="33" t="s">
-        <v>313</v>
+      <c r="D23" s="29" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>252</v>
-      </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
+        <v>247</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="B25" s="33" t="s">
-        <v>314</v>
-      </c>
-      <c r="C25" s="33" t="b">
+        <v>248</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="C25" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="D25" s="33" t="s">
-        <v>315</v>
+      <c r="D25" s="29" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>254</v>
-      </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
+        <v>249</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="B27" s="33" t="s">
-        <v>293</v>
-      </c>
-      <c r="C27" s="33" t="b">
+        <v>288</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="C27" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="D27" s="33" t="s">
-        <v>316</v>
+      <c r="D27" s="29" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="B28" s="33" t="s">
-        <v>294</v>
-      </c>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
+        <v>289</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>295</v>
-      </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
+        <v>290</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
-        <v>296</v>
-      </c>
-      <c r="B30" s="33" t="s">
-        <v>296</v>
-      </c>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+        <v>291</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>297</v>
-      </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
+        <v>292</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
-        <v>298</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>298</v>
-      </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
+        <v>293</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>299</v>
-      </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+        <v>294</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="26" t="s">
-        <v>300</v>
-      </c>
-      <c r="B34" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
+        <v>295</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
     </row>
     <row r="35" spans="1:4" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
+        <v>296</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
+      <c r="A36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4963,72 +5003,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>40</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>